<commit_message>
Larger update with steady state approximation
</commit_message>
<xml_diff>
--- a/Epsilon.xlsx
+++ b/Epsilon.xlsx
@@ -386,7 +386,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +396,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -431,11 +432,11 @@
         <v>0.7</v>
       </c>
       <c r="B3">
-        <v>0.32640000000000002</v>
+        <v>0.32829999999999998</v>
       </c>
       <c r="C3">
         <f>B3^(D3/30)</f>
-        <v>0.68852024829052638</v>
+        <v>0.68985364115511338</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -445,11 +446,11 @@
       </c>
       <c r="F3">
         <f>A3*C3*(E3-D3)/E3</f>
-        <v>0.26823283287061078</v>
+        <v>0.26875229434801201</v>
       </c>
       <c r="G3">
         <f>(1-F3)/(1+F3)</f>
-        <v>0.57699749459494287</v>
+        <v>0.57635182920221817</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -483,11 +484,11 @@
       </c>
       <c r="B7">
         <f>B3</f>
-        <v>0.32640000000000002</v>
+        <v>0.32829999999999998</v>
       </c>
       <c r="C7">
         <f>B7^(D7/30)</f>
-        <v>0.82977120237480306</v>
+        <v>0.830574283947627</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -497,11 +498,11 @@
       </c>
       <c r="F7">
         <f>A7*C7*(E7-D7)/E7</f>
-        <v>0.37985719748853441</v>
+        <v>0.38022483656149153</v>
       </c>
       <c r="G7">
         <f>(1-F7)/(1+F7)</f>
-        <v>0.44942534897102537</v>
+        <v>0.44903927752998113</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -512,7 +513,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>(G3+G7)/2</f>
-        <v>0.51321142178298418</v>
+        <v>0.51269555336609962</v>
       </c>
     </row>
   </sheetData>

</xml_diff>